<commit_message>
fim after pulling haver
</commit_message>
<xml_diff>
--- a/comparison_levels.xlsx
+++ b/comparison_levels.xlsx
@@ -494,7 +494,7 @@
         <v>283.95</v>
       </c>
       <c r="E2" t="n">
-        <v>321.36</v>
+        <v>833.48736</v>
       </c>
     </row>
     <row r="3">
@@ -511,7 +511,7 @@
         <v>291.4</v>
       </c>
       <c r="E3" t="n">
-        <v>287.128</v>
+        <v>772.713928</v>
       </c>
     </row>
     <row r="4">
@@ -528,7 +528,7 @@
         <v>294.149</v>
       </c>
       <c r="E4" t="n">
-        <v>285.907</v>
+        <v>797.587807</v>
       </c>
     </row>
     <row r="5">
@@ -545,7 +545,7 @@
         <v>322.636796</v>
       </c>
       <c r="E5" t="n">
-        <v>312.437</v>
+        <v>835.976837</v>
       </c>
     </row>
     <row r="6">
@@ -562,7 +562,7 @@
         <v>324.527743184</v>
       </c>
       <c r="E6" t="n">
-        <v>399.868503114219</v>
+        <v>944.349933594219</v>
       </c>
     </row>
     <row r="7">
@@ -579,7 +579,7 @@
         <v>319.321854156736</v>
       </c>
       <c r="E7" t="n">
-        <v>398.057230799068</v>
+        <v>964.317918498268</v>
       </c>
     </row>
     <row r="8">
@@ -596,7 +596,7 @@
         <v>319.119141573363</v>
       </c>
       <c r="E8" t="n">
-        <v>387.959508195506</v>
+        <v>976.870623402674</v>
       </c>
     </row>
     <row r="9">
@@ -613,7 +613,7 @@
         <v>309.919618139656</v>
       </c>
       <c r="E9" t="n">
-        <v>391.981848050487</v>
+        <v>1004.44940786594</v>
       </c>
     </row>
     <row r="10">
@@ -630,7 +630,7 @@
         <v>310.723296612215</v>
       </c>
       <c r="E10" t="n">
-        <v>450.714132717849</v>
+        <v>1087.68039492592</v>
       </c>
     </row>
     <row r="11">
@@ -647,7 +647,7 @@
         <v>311.530189798664</v>
       </c>
       <c r="E11" t="n">
-        <v>463.649847371906</v>
+        <v>1126.0947600683</v>
       </c>
     </row>
     <row r="12">
@@ -664,7 +664,7 @@
         <v>312.340310557859</v>
       </c>
       <c r="E12" t="n">
-        <v>460.949906285691</v>
+        <v>1149.89261548994</v>
       </c>
     </row>
     <row r="13">
@@ -681,7 +681,7 @@
         <v>313.15367180009</v>
       </c>
       <c r="E13" t="n">
-        <v>473.509054137119</v>
+        <v>1190.00947170954</v>
       </c>
     </row>
     <row r="14">
@@ -953,7 +953,7 @@
         <v>250.9</v>
       </c>
       <c r="E29" t="n">
-        <v>250.9</v>
+        <v>254.1</v>
       </c>
     </row>
     <row r="30">
@@ -970,7 +970,7 @@
         <v>234.947544234898</v>
       </c>
       <c r="E30" t="n">
-        <v>223.257122416534</v>
+        <v>226.104562798092</v>
       </c>
     </row>
     <row r="31">
@@ -987,7 +987,7 @@
         <v>218.995088469796</v>
       </c>
       <c r="E31" t="n">
-        <v>220.813938791733</v>
+        <v>223.630218600954</v>
       </c>
     </row>
     <row r="32">
@@ -1004,7 +1004,7 @@
         <v>248.343882535097</v>
       </c>
       <c r="E32" t="n">
-        <v>223.356844197138</v>
+        <v>226.205556438792</v>
       </c>
     </row>
     <row r="33">
@@ -1021,7 +1021,7 @@
         <v>277.692676600398</v>
       </c>
       <c r="E33" t="n">
-        <v>247.115150796183</v>
+        <v>250.266878506616</v>
       </c>
     </row>
     <row r="34">
@@ -1038,7 +1038,7 @@
         <v>307.041470665698</v>
       </c>
       <c r="E34" t="n">
-        <v>252.284468479196</v>
+        <v>255.502126108265</v>
       </c>
     </row>
     <row r="35">
@@ -1055,7 +1055,7 @@
         <v>336.390264730999</v>
       </c>
       <c r="E35" t="n">
-        <v>257.029357973499</v>
+        <v>260.307532327884</v>
       </c>
     </row>
     <row r="36">
@@ -1072,7 +1072,7 @@
         <v>353.748434918633</v>
       </c>
       <c r="E36" t="n">
-        <v>262.002785723261</v>
+        <v>265.344391599365</v>
       </c>
     </row>
     <row r="37">
@@ -1089,7 +1089,7 @@
         <v>371.106605106268</v>
       </c>
       <c r="E37" t="n">
-        <v>285.295054377787</v>
+        <v>288.933731834977</v>
       </c>
     </row>
     <row r="38">
@@ -1157,7 +1157,7 @@
         <v>3421.7</v>
       </c>
       <c r="E41" t="n">
-        <v>3421.7</v>
+        <v>3422.5</v>
       </c>
     </row>
     <row r="42">
@@ -1174,7 +1174,7 @@
         <v>3453.78646361648</v>
       </c>
       <c r="E42" t="n">
-        <v>3474.18790303048</v>
+        <v>3475.0001727918</v>
       </c>
     </row>
     <row r="43">
@@ -1191,7 +1191,7 @@
         <v>3485.87292723296</v>
       </c>
       <c r="E43" t="n">
-        <v>3543.77666326433</v>
+        <v>3544.60504209738</v>
       </c>
     </row>
     <row r="44">
@@ -1208,7 +1208,7 @@
         <v>3588.41167220364</v>
       </c>
       <c r="E44" t="n">
-        <v>3579.61259173013</v>
+        <v>3580.44946756899</v>
       </c>
     </row>
     <row r="45">
@@ -1225,7 +1225,7 @@
         <v>3690.95041717432</v>
       </c>
       <c r="E45" t="n">
-        <v>3664.28349282268</v>
+        <v>3665.14221657143</v>
       </c>
     </row>
     <row r="46">
@@ -1242,7 +1242,7 @@
         <v>3793.489162145</v>
       </c>
       <c r="E46" t="n">
-        <v>3697.69275074661</v>
+        <v>3698.55945820078</v>
       </c>
     </row>
     <row r="47">
@@ -1259,7 +1259,7 @@
         <v>3896.02790711568</v>
       </c>
       <c r="E47" t="n">
-        <v>3735.24793281616</v>
+        <v>3736.12351960347</v>
       </c>
     </row>
     <row r="48">
@@ -1276,7 +1276,7 @@
         <v>3937.83567156767</v>
       </c>
       <c r="E48" t="n">
-        <v>3771.79254794261</v>
+        <v>3772.67679205759</v>
       </c>
     </row>
     <row r="49">
@@ -1293,7 +1293,7 @@
         <v>3979.64343601966</v>
       </c>
       <c r="E49" t="n">
-        <v>3853.5609205575</v>
+        <v>3854.46108192878</v>
       </c>
     </row>
     <row r="50">
@@ -1769,7 +1769,7 @@
         <v>1557.2</v>
       </c>
       <c r="E77" t="n">
-        <v>1557.2</v>
+        <v>1557.1</v>
       </c>
     </row>
     <row r="78">
@@ -1786,7 +1786,7 @@
         <v>1577.25764129727</v>
       </c>
       <c r="E78" t="n">
-        <v>1611.71407644456</v>
+        <v>1611.61604692514</v>
       </c>
     </row>
     <row r="79">
@@ -1803,7 +1803,7 @@
         <v>1621.76252088349</v>
       </c>
       <c r="E79" t="n">
-        <v>1657.10842408159</v>
+        <v>1657.01079302431</v>
       </c>
     </row>
     <row r="80">
@@ -1820,7 +1820,7 @@
         <v>1636.28609206765</v>
       </c>
       <c r="E80" t="n">
-        <v>1694.55160283856</v>
+        <v>1694.45397666319</v>
       </c>
     </row>
     <row r="81">
@@ -1837,7 +1837,7 @@
         <v>1652.21322446296</v>
       </c>
       <c r="E81" t="n">
-        <v>1686.03145368921</v>
+        <v>1685.93358290488</v>
       </c>
     </row>
     <row r="82">
@@ -1854,7 +1854,7 @@
         <v>1677.99830822929</v>
       </c>
       <c r="E82" t="n">
-        <v>1661.12351738379</v>
+        <v>1661.02549111116</v>
       </c>
     </row>
     <row r="83">
@@ -1871,7 +1871,7 @@
         <v>1703.86907168331</v>
       </c>
       <c r="E83" t="n">
-        <v>1639.91290155898</v>
+        <v>1639.81448236417</v>
       </c>
     </row>
     <row r="84">
@@ -1888,7 +1888,7 @@
         <v>1720.06699818956</v>
       </c>
       <c r="E84" t="n">
-        <v>1642.83125317135</v>
+        <v>1642.73245479907</v>
       </c>
     </row>
     <row r="85">
@@ -1905,7 +1905,7 @@
         <v>1736.26780409165</v>
       </c>
       <c r="E85" t="n">
-        <v>1648.88020614518</v>
+        <v>1648.78101932228</v>
       </c>
     </row>
     <row r="86">
@@ -1973,7 +1973,7 @@
         <v>2008.1</v>
       </c>
       <c r="E89" t="n">
-        <v>2008.1</v>
+        <v>2008.9</v>
       </c>
     </row>
     <row r="90">
@@ -1990,7 +1990,7 @@
         <v>1830.5942369875</v>
       </c>
       <c r="E90" t="n">
-        <v>1743.25233333333</v>
+        <v>1725.23333333333</v>
       </c>
     </row>
     <row r="91">
@@ -2007,7 +2007,7 @@
         <v>1748.67185118644</v>
       </c>
       <c r="E91" t="n">
-        <v>1719.419</v>
+        <v>1701.4</v>
       </c>
     </row>
     <row r="92">
@@ -2024,7 +2024,7 @@
         <v>1744.82714721481</v>
       </c>
       <c r="E92" t="n">
-        <v>1695.58566666667</v>
+        <v>1677.56666666667</v>
       </c>
     </row>
     <row r="93">
@@ -2041,7 +2041,7 @@
         <v>1746.33089386998</v>
       </c>
       <c r="E93" t="n">
-        <v>1751.41089578671</v>
+        <v>1732.45226943615</v>
       </c>
     </row>
     <row r="94">
@@ -2058,7 +2058,7 @@
         <v>1739.72729546593</v>
       </c>
       <c r="E94" t="n">
-        <v>1742.57756245338</v>
+        <v>1723.61893610282</v>
       </c>
     </row>
     <row r="95">
@@ -2075,7 +2075,7 @@
         <v>1720.9927258959</v>
       </c>
       <c r="E95" t="n">
-        <v>1738.74422912005</v>
+        <v>1719.78560276948</v>
       </c>
     </row>
     <row r="96">
@@ -2092,7 +2092,7 @@
         <v>1743.15353220976</v>
       </c>
       <c r="E96" t="n">
-        <v>1734.91089578671</v>
+        <v>1715.95226943615</v>
       </c>
     </row>
     <row r="97">
@@ -2109,7 +2109,7 @@
         <v>1754.69385584676</v>
       </c>
       <c r="E97" t="n">
-        <v>1807.85861292016</v>
+        <v>1787.82528072634</v>
       </c>
     </row>
     <row r="98">
@@ -2789,7 +2789,7 @@
         <v>694.4</v>
       </c>
       <c r="E137" t="n">
-        <v>694.4</v>
+        <v>700.1</v>
       </c>
     </row>
     <row r="138">
@@ -2806,7 +2806,7 @@
         <v>700.781947651713</v>
       </c>
       <c r="E138" t="n">
-        <v>702.833823132627</v>
+        <v>709.317033670381</v>
       </c>
     </row>
     <row r="139">
@@ -2823,7 +2823,7 @@
         <v>707.22254918567</v>
       </c>
       <c r="E139" t="n">
-        <v>709.284503744743</v>
+        <v>716.556958472619</v>
       </c>
     </row>
     <row r="140">
@@ -2840,7 +2840,7 @@
         <v>714.408373429083</v>
       </c>
       <c r="E140" t="n">
-        <v>716.425540083115</v>
+        <v>723.601712301784</v>
       </c>
     </row>
     <row r="141">
@@ -2857,7 +2857,7 @@
         <v>721.667210149427</v>
       </c>
       <c r="E141" t="n">
-        <v>723.645276465573</v>
+        <v>730.722545030267</v>
       </c>
     </row>
     <row r="142">
@@ -2874,7 +2874,7 @@
         <v>728.999801199216</v>
       </c>
       <c r="E142" t="n">
-        <v>730.931247090814</v>
+        <v>737.906900714206</v>
       </c>
     </row>
     <row r="143">
@@ -2891,7 +2891,7 @@
         <v>736.406895968652</v>
       </c>
       <c r="E143" t="n">
-        <v>738.529123240845</v>
+        <v>745.392187430077</v>
       </c>
     </row>
     <row r="144">
@@ -2908,7 +2908,7 @@
         <v>743.759624360676</v>
       </c>
       <c r="E144" t="n">
-        <v>746.011559486059</v>
+        <v>752.35382628783</v>
       </c>
     </row>
     <row r="145">
@@ -2925,7 +2925,7 @@
         <v>751.185766805586</v>
       </c>
       <c r="E145" t="n">
-        <v>752.889318349495</v>
+        <v>758.700123139062</v>
       </c>
     </row>
     <row r="146">
@@ -3010,7 +3010,7 @@
         <v>527.956732288882</v>
       </c>
       <c r="E150" t="n">
-        <v>535.104721704335</v>
+        <v>537.804464289892</v>
       </c>
     </row>
     <row r="151">
@@ -3027,7 +3027,7 @@
         <v>531.805697673386</v>
       </c>
       <c r="E151" t="n">
-        <v>540.015967492657</v>
+        <v>543.293778228426</v>
       </c>
     </row>
     <row r="152">
@@ -3044,7 +3044,7 @@
         <v>537.209176789722</v>
       </c>
       <c r="E152" t="n">
-        <v>545.452817764736</v>
+        <v>548.635113455558</v>
       </c>
     </row>
     <row r="153">
@@ -3061,7 +3061,7 @@
         <v>542.667558639685</v>
       </c>
       <c r="E153" t="n">
-        <v>550.352871403991</v>
+        <v>553.435140096838</v>
       </c>
     </row>
     <row r="154">
@@ -3078,7 +3078,7 @@
         <v>548.18140106945</v>
       </c>
       <c r="E154" t="n">
-        <v>555.894059863275</v>
+        <v>558.876432310261</v>
       </c>
     </row>
     <row r="155">
@@ -3095,7 +3095,7 @@
         <v>553.75126759326</v>
       </c>
       <c r="E155" t="n">
-        <v>503.135749319218</v>
+        <v>507.751066023249</v>
       </c>
     </row>
     <row r="156">
@@ -3112,7 +3112,7 @@
         <v>500.361978997004</v>
       </c>
       <c r="E156" t="n">
-        <v>505.571760580738</v>
+        <v>509.847048815395</v>
       </c>
     </row>
     <row r="157">
@@ -3129,7 +3129,7 @@
         <v>505.357893279448</v>
       </c>
       <c r="E157" t="n">
-        <v>510.232815242991</v>
+        <v>514.147739005903</v>
       </c>
     </row>
     <row r="158">
@@ -3809,7 +3809,7 @@
         <v>96.6</v>
       </c>
       <c r="E197" t="n">
-        <v>96.6</v>
+        <v>101.2</v>
       </c>
     </row>
     <row r="198">
@@ -3826,7 +3826,7 @@
         <v>97.5902750001144</v>
       </c>
       <c r="E198" t="n">
-        <v>85.957106518283</v>
+        <v>90.0503020667727</v>
       </c>
     </row>
     <row r="199">
@@ -3843,7 +3843,7 @@
         <v>99.0031852234919</v>
       </c>
       <c r="E199" t="n">
-        <v>85.0164467408585</v>
+        <v>89.0648489666137</v>
       </c>
     </row>
     <row r="200">
@@ -3860,7 +3860,7 @@
         <v>100.319278382126</v>
       </c>
       <c r="E200" t="n">
-        <v>85.9955007949126</v>
+        <v>90.0905246422893</v>
       </c>
     </row>
     <row r="201">
@@ -3877,7 +3877,7 @@
         <v>101.564637612181</v>
       </c>
       <c r="E201" t="n">
-        <v>87.1818839427663</v>
+        <v>91.3334022257552</v>
       </c>
     </row>
     <row r="202">
@@ -3894,7 +3894,7 @@
         <v>102.592932098907</v>
       </c>
       <c r="E202" t="n">
-        <v>89.0056120826709</v>
+        <v>93.2439745627981</v>
       </c>
     </row>
     <row r="203">
@@ -3911,7 +3911,7 @@
         <v>103.696823471802</v>
       </c>
       <c r="E203" t="n">
-        <v>90.6796025437202</v>
+        <v>94.9976788553259</v>
       </c>
     </row>
     <row r="204">
@@ -3928,7 +3928,7 @@
         <v>104.786125971928</v>
       </c>
       <c r="E204" t="n">
-        <v>92.4342209856916</v>
+        <v>96.8358505564388</v>
       </c>
     </row>
     <row r="205">
@@ -3945,7 +3945,7 @@
         <v>105.788779409544</v>
       </c>
       <c r="E205" t="n">
-        <v>93.7242686804451</v>
+        <v>98.1873290937997</v>
       </c>
     </row>
     <row r="206">
@@ -4013,7 +4013,7 @@
         <v>1965.1</v>
       </c>
       <c r="E209" t="n">
-        <v>1965.1</v>
+        <v>1951.9</v>
       </c>
     </row>
     <row r="210">
@@ -4030,7 +4030,7 @@
         <v>1985.24481783359</v>
       </c>
       <c r="E210" t="n">
-        <v>1991.85744933556</v>
+        <v>1978.53353532519</v>
       </c>
     </row>
     <row r="211">
@@ -4047,7 +4047,7 @@
         <v>2013.98715613545</v>
       </c>
       <c r="E211" t="n">
-        <v>2025.43992024315</v>
+        <v>2011.95360806146</v>
       </c>
     </row>
     <row r="212">
@@ -4064,7 +4064,7 @@
         <v>2040.75997876518</v>
       </c>
       <c r="E212" t="n">
-        <v>2049.19991593418</v>
+        <v>2035.53278727767</v>
       </c>
     </row>
     <row r="213">
@@ -4081,7 +4081,7 @@
         <v>2066.09388583537</v>
       </c>
       <c r="E213" t="n">
-        <v>2075.34687053198</v>
+        <v>2061.48596715345</v>
       </c>
     </row>
     <row r="214">
@@ -4098,7 +4098,7 @@
         <v>2087.01212078221</v>
       </c>
       <c r="E214" t="n">
-        <v>2097.72813772305</v>
+        <v>2083.69984430965</v>
       </c>
     </row>
     <row r="215">
@@ -4115,7 +4115,7 @@
         <v>2109.46819673332</v>
       </c>
       <c r="E215" t="n">
-        <v>2120.88842016622</v>
+        <v>2106.69406718421</v>
       </c>
     </row>
     <row r="216">
@@ -4132,7 +4132,7 @@
         <v>2131.62749635026</v>
       </c>
       <c r="E216" t="n">
-        <v>2143.86300996835</v>
+        <v>2129.50119350236</v>
       </c>
     </row>
     <row r="217">
@@ -4149,7 +4149,7 @@
         <v>2152.02412440678</v>
       </c>
       <c r="E217" t="n">
-        <v>2165.72381547559</v>
+        <v>2151.20880788586</v>
       </c>
     </row>
     <row r="218">
@@ -4217,7 +4217,7 @@
         <v>2389.4</v>
       </c>
       <c r="E221" t="n">
-        <v>2389.4</v>
+        <v>2389.6</v>
       </c>
     </row>
     <row r="222">
@@ -4234,7 +4234,7 @@
         <v>2447.0172484966</v>
       </c>
       <c r="E222" t="n">
-        <v>2441.43678535797</v>
+        <v>2441.64114099415</v>
       </c>
     </row>
     <row r="223">
@@ -4251,7 +4251,7 @@
         <v>2494.55434408433</v>
       </c>
       <c r="E223" t="n">
-        <v>2505.9720828605</v>
+        <v>2506.18184029607</v>
       </c>
     </row>
     <row r="224">
@@ -4268,7 +4268,7 @@
         <v>2534.13864336425</v>
       </c>
       <c r="E224" t="n">
-        <v>2577.98706646957</v>
+        <v>2578.20285177688</v>
       </c>
     </row>
     <row r="225">
@@ -4285,7 +4285,7 @@
         <v>2574.35107758667</v>
       </c>
       <c r="E225" t="n">
-        <v>2628.06845314526</v>
+        <v>2634.35141978861</v>
       </c>
     </row>
     <row r="226">
@@ -4302,7 +4302,7 @@
         <v>2615.20161417587</v>
       </c>
       <c r="E226" t="n">
-        <v>2669.77139178842</v>
+        <v>2685.52777121801</v>
       </c>
     </row>
     <row r="227">
@@ -4319,7 +4319,7 @@
         <v>2653.57667992124</v>
       </c>
       <c r="E227" t="n">
-        <v>2708.94720649701</v>
+        <v>2731.33891384639</v>
       </c>
     </row>
     <row r="228">
@@ -4336,7 +4336,7 @@
         <v>2689.33408740552</v>
       </c>
       <c r="E228" t="n">
-        <v>2745.45074265667</v>
+        <v>2768.14418216863</v>
       </c>
     </row>
     <row r="229">
@@ -4353,7 +4353,7 @@
         <v>2722.33822463033</v>
       </c>
       <c r="E229" t="n">
-        <v>2779.14355778394</v>
+        <v>2802.11549650558</v>
       </c>
     </row>
     <row r="230">
@@ -4438,7 +4438,7 @@
         <v>157.035442282325</v>
       </c>
       <c r="E234" t="n">
-        <v>106.462467400266</v>
+        <v>103.107612369063</v>
       </c>
     </row>
     <row r="235">
@@ -4455,7 +4455,7 @@
         <v>168.865956762063</v>
       </c>
       <c r="E235" t="n">
-        <v>95.4839256275397</v>
+        <v>90.6057100111654</v>
       </c>
     </row>
     <row r="236">
@@ -4472,7 +4472,7 @@
         <v>165.254970796809</v>
       </c>
       <c r="E236" t="n">
-        <v>85.6375047082815</v>
+        <v>79.619675967694</v>
       </c>
     </row>
     <row r="237">
@@ -4489,7 +4489,7 @@
         <v>161.948480308013</v>
       </c>
       <c r="E237" t="n">
-        <v>76.8064589349655</v>
+        <v>69.9657096712712</v>
       </c>
     </row>
     <row r="238">
@@ -4506,7 +4506,7 @@
         <v>167.470445884562</v>
       </c>
       <c r="E238" t="n">
-        <v>68.8860815623236</v>
+        <v>61.4822965593436</v>
       </c>
     </row>
     <row r="239">
@@ -4523,7 +4523,7 @@
         <v>172.158013427143</v>
       </c>
       <c r="E239" t="n">
-        <v>61.7824633346147</v>
+        <v>54.0275058735411</v>
       </c>
     </row>
     <row r="240">
@@ -4540,7 +4540,7 @@
         <v>174.763537539673</v>
       </c>
       <c r="E240" t="n">
-        <v>55.4113790351041</v>
+        <v>47.476616103598</v>
       </c>
     </row>
     <row r="241">
@@ -4557,7 +4557,7 @@
         <v>176.450477307304</v>
       </c>
       <c r="E241" t="n">
-        <v>49.6972888559417</v>
+        <v>41.7200283486025</v>
       </c>
     </row>
     <row r="242">

</xml_diff>